<commit_message>
Reorganized information. Added Exception Catching and logging
</commit_message>
<xml_diff>
--- a/testcases/KeywordDrivenFramework-2.xlsx
+++ b/testcases/KeywordDrivenFramework-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500"/>
+    <workbookView xWindow="-31280" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ContactUs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="142">
   <si>
     <t>TCName</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Submit Google Address</t>
   </si>
   <si>
-    <t>quit</t>
-  </si>
-  <si>
     <t>Param2</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>Uniforms</t>
   </si>
   <si>
-    <t>Verify Search Results Available</t>
-  </si>
-  <si>
     <t>CA Search</t>
   </si>
   <si>
@@ -406,9 +400,6 @@
     <t>Verify URL</t>
   </si>
   <si>
-    <t>driver</t>
-  </si>
-  <si>
     <t>Contact Us CA</t>
   </si>
   <si>
@@ -446,13 +437,25 @@
   </si>
   <si>
     <t>Merci. Nous avons reçu votre demande. Un représentant du service à la clientèle communiquera avec vous d’ici 48 heures. Nous vous remercions de votre intérêt pour Cintas, et serons heureux de discuter avec vous bientôt.</t>
+  </si>
+  <si>
+    <t>Take Screenshot</t>
+  </si>
+  <si>
+    <t>Verify Search Results Available US</t>
+  </si>
+  <si>
+    <t>Verify Search Results Available CA</t>
+  </si>
+  <si>
+    <t>Verify Search Results Available CA/FR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -485,6 +488,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -503,9 +514,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -528,7 +543,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -859,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -896,12 +915,12 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -915,7 +934,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1166,7 +1185,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1186,7 +1205,7 @@
         <v>25</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1206,7 +1225,7 @@
         <v>26</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1271,7 +1290,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
@@ -1283,68 +1302,62 @@
         <v>49</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="B25">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="B28">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
@@ -1353,15 +1366,15 @@
         <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
         <v>38</v>
@@ -1370,15 +1383,15 @@
         <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
         <v>38</v>
@@ -1387,15 +1400,15 @@
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
@@ -1404,15 +1417,15 @@
         <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
         <v>38</v>
@@ -1421,15 +1434,15 @@
         <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="B33">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D33" t="s">
         <v>38</v>
@@ -1438,16 +1451,15 @@
         <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="1"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
       <c r="B34">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
         <v>38</v>
@@ -1456,53 +1468,51 @@
         <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10">
       <c r="B35">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:10">
       <c r="B36">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="B37">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -1511,18 +1521,18 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="B38">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1531,18 +1541,18 @@
         <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="B39">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
         <v>15</v>
@@ -1551,18 +1561,18 @@
         <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="B40">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
         <v>15</v>
@@ -1571,18 +1581,18 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="B41">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1591,18 +1601,18 @@
         <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="2">
-        <v>45324</v>
+        <v>25</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="B42">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
@@ -1611,18 +1621,18 @@
         <v>12</v>
       </c>
       <c r="F42" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
+      </c>
+      <c r="G42" s="2">
+        <v>45324</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="B43">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
@@ -1631,35 +1641,38 @@
         <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>31</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="B44">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="B45">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -1668,91 +1681,91 @@
         <v>12</v>
       </c>
       <c r="F45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="B46">
+        <v>42</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30">
-      <c r="B46">
+    <row r="47" spans="1:10" ht="30">
+      <c r="B47">
         <v>43</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C47" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" t="s">
         <v>51</v>
       </c>
-      <c r="E46" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
+    <row r="48" spans="1:10">
+      <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="B48">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="49" spans="2:7">
       <c r="B49">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="2:7">
       <c r="B50">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="2:7">
       <c r="B51">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
         <v>38</v>
@@ -1761,15 +1774,15 @@
         <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="2:7">
       <c r="B52">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" t="s">
         <v>38</v>
@@ -1778,15 +1791,15 @@
         <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:7">
       <c r="B53">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D53" t="s">
         <v>38</v>
@@ -1795,15 +1808,15 @@
         <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="2:7">
       <c r="B54">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
         <v>38</v>
@@ -1812,15 +1825,15 @@
         <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="2:7">
       <c r="B55">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
         <v>38</v>
@@ -1829,15 +1842,15 @@
         <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="2:7">
       <c r="B56">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
         <v>38</v>
@@ -1846,15 +1859,15 @@
         <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="2:7">
       <c r="B57">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D57" t="s">
         <v>38</v>
@@ -1863,53 +1876,50 @@
         <v>12</v>
       </c>
       <c r="F57" t="s">
-        <v>31</v>
-      </c>
-      <c r="G57" s="3"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="58" spans="2:7">
       <c r="B58">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G58" s="3"/>
     </row>
     <row r="59" spans="2:7">
       <c r="B59">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>16</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="2:7">
       <c r="B60">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D60" t="s">
         <v>15</v>
@@ -1918,18 +1928,18 @@
         <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D61" t="s">
         <v>15</v>
@@ -1938,18 +1948,18 @@
         <v>12</v>
       </c>
       <c r="F61" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="2:7">
       <c r="B62">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
         <v>15</v>
@@ -1958,18 +1968,18 @@
         <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="2:7">
       <c r="B63">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
         <v>15</v>
@@ -1978,18 +1988,18 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="2:7">
       <c r="B64">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
@@ -1998,18 +2008,18 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>26</v>
-      </c>
-      <c r="G64" s="2">
-        <v>45324</v>
+        <v>25</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="B65">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D65" t="s">
         <v>15</v>
@@ -2018,18 +2028,18 @@
         <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>29</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
+      </c>
+      <c r="G65" s="2">
+        <v>45324</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="B66">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -2038,35 +2048,38 @@
         <v>12</v>
       </c>
       <c r="F66" t="s">
-        <v>31</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="B67">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="B68">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -2075,32 +2088,32 @@
         <v>12</v>
       </c>
       <c r="F68" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E69" t="s">
         <v>12</v>
       </c>
       <c r="F69" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="B70">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D70" t="s">
         <v>38</v>
@@ -2109,35 +2122,32 @@
         <v>12</v>
       </c>
       <c r="F70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="B71">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E71" t="s">
         <v>12</v>
       </c>
       <c r="F71" t="s">
-        <v>25</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="B72">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D72" t="s">
         <v>15</v>
@@ -2146,122 +2156,125 @@
         <v>12</v>
       </c>
       <c r="F72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="B73">
+        <v>69</v>
+      </c>
+      <c r="C73" t="s">
+        <v>28</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="B74">
         <v>70</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>56</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>11</v>
       </c>
-      <c r="E73" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30">
-      <c r="B74">
+    <row r="75" spans="1:7" ht="30">
+      <c r="B75">
         <v>71</v>
       </c>
-      <c r="C74" t="s">
-        <v>137</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="C75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D75" t="s">
         <v>51</v>
       </c>
-      <c r="E74" t="s">
-        <v>12</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" t="s">
         <v>49</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="B75">
+    <row r="76" spans="1:7">
+      <c r="B76">
         <v>72</v>
       </c>
-      <c r="C75" t="s">
-        <v>139</v>
-      </c>
-      <c r="D75" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76">
+      <c r="C76" t="s">
+        <v>136</v>
+      </c>
+      <c r="D76" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77">
         <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="B77">
-        <v>74</v>
-      </c>
-      <c r="C77" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="B79">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C79" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
       </c>
       <c r="F79" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="B80">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D80" t="s">
         <v>38</v>
@@ -2270,15 +2283,15 @@
         <v>12</v>
       </c>
       <c r="F80" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="2:7">
       <c r="B81">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D81" t="s">
         <v>38</v>
@@ -2287,15 +2300,15 @@
         <v>12</v>
       </c>
       <c r="F81" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="2:7">
       <c r="B82">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C82" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D82" t="s">
         <v>38</v>
@@ -2304,15 +2317,15 @@
         <v>12</v>
       </c>
       <c r="F82" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="2:7">
       <c r="B83">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
         <v>38</v>
@@ -2321,15 +2334,15 @@
         <v>12</v>
       </c>
       <c r="F83" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="2:7">
       <c r="B84">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D84" t="s">
         <v>38</v>
@@ -2338,15 +2351,15 @@
         <v>12</v>
       </c>
       <c r="F84" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85" spans="2:7">
       <c r="B85">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D85" t="s">
         <v>38</v>
@@ -2355,15 +2368,15 @@
         <v>12</v>
       </c>
       <c r="F85" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="2:7">
       <c r="B86">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D86" t="s">
         <v>38</v>
@@ -2372,53 +2385,50 @@
         <v>12</v>
       </c>
       <c r="F86" t="s">
-        <v>31</v>
-      </c>
-      <c r="G86" s="3"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="87" spans="2:7">
       <c r="B87">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C87" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D87" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E87" t="s">
         <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G87" s="3"/>
     </row>
     <row r="88" spans="2:7">
       <c r="B88">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E88" t="s">
         <v>12</v>
       </c>
       <c r="F88" t="s">
-        <v>16</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="2:7">
       <c r="B89">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D89" t="s">
         <v>15</v>
@@ -2427,18 +2437,18 @@
         <v>12</v>
       </c>
       <c r="F89" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" spans="2:7">
       <c r="B90">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C90" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D90" t="s">
         <v>15</v>
@@ -2447,18 +2457,18 @@
         <v>12</v>
       </c>
       <c r="F90" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="2:7">
       <c r="B91">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D91" t="s">
         <v>15</v>
@@ -2467,18 +2477,18 @@
         <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="2:7">
       <c r="B92">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D92" t="s">
         <v>15</v>
@@ -2487,18 +2497,18 @@
         <v>12</v>
       </c>
       <c r="F92" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>129</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="2:7">
       <c r="B93">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D93" t="s">
         <v>15</v>
@@ -2507,18 +2517,18 @@
         <v>12</v>
       </c>
       <c r="F93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="2:7">
       <c r="B94">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D94" t="s">
         <v>15</v>
@@ -2527,18 +2537,18 @@
         <v>12</v>
       </c>
       <c r="F94" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="2:7">
       <c r="B95">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D95" t="s">
         <v>15</v>
@@ -2547,111 +2557,114 @@
         <v>12</v>
       </c>
       <c r="F95" t="s">
-        <v>31</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="2:7">
       <c r="B96">
+        <v>92</v>
+      </c>
+      <c r="C96" t="s">
+        <v>30</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" t="s">
+        <v>31</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="B97">
         <v>93</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>36</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>11</v>
       </c>
-      <c r="E96" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="30">
-      <c r="B97">
+    <row r="98" spans="1:7" ht="30">
+      <c r="B98">
         <v>94</v>
       </c>
-      <c r="C97" t="s">
-        <v>135</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C98" t="s">
+        <v>132</v>
+      </c>
+      <c r="D98" t="s">
         <v>51</v>
       </c>
-      <c r="E97" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" t="s">
         <v>49</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>131</v>
-      </c>
-      <c r="B98">
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>128</v>
+      </c>
+      <c r="B99">
         <v>95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="B99">
-        <v>96</v>
-      </c>
-      <c r="C99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" t="s">
-        <v>9</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="B100">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D100" t="s">
-        <v>11</v>
-      </c>
-      <c r="E100" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="B101">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C101" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D101" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E101" t="s">
         <v>12</v>
       </c>
       <c r="F101" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="B102">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D102" t="s">
         <v>38</v>
@@ -2660,15 +2673,15 @@
         <v>12</v>
       </c>
       <c r="F102" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="B103">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C103" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D103" t="s">
         <v>38</v>
@@ -2677,15 +2690,15 @@
         <v>12</v>
       </c>
       <c r="F103" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="B104">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C104" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D104" t="s">
         <v>38</v>
@@ -2694,15 +2707,15 @@
         <v>12</v>
       </c>
       <c r="F104" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="B105">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D105" t="s">
         <v>38</v>
@@ -2711,15 +2724,15 @@
         <v>12</v>
       </c>
       <c r="F105" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="B106">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C106" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D106" t="s">
         <v>38</v>
@@ -2728,15 +2741,15 @@
         <v>12</v>
       </c>
       <c r="F106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="B107">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D107" t="s">
         <v>38</v>
@@ -2745,15 +2758,15 @@
         <v>12</v>
       </c>
       <c r="F107" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="B108">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C108" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D108" t="s">
         <v>38</v>
@@ -2762,53 +2775,50 @@
         <v>12</v>
       </c>
       <c r="F108" t="s">
-        <v>31</v>
-      </c>
-      <c r="G108" s="3"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="109" spans="1:7">
       <c r="B109">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E109" t="s">
         <v>12</v>
       </c>
       <c r="F109" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G109" s="3"/>
     </row>
     <row r="110" spans="1:7">
       <c r="B110">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D110" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E110" t="s">
         <v>12</v>
       </c>
       <c r="F110" t="s">
-        <v>16</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="B111">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D111" t="s">
         <v>15</v>
@@ -2817,18 +2827,18 @@
         <v>12</v>
       </c>
       <c r="F111" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="B112">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D112" t="s">
         <v>15</v>
@@ -2837,18 +2847,18 @@
         <v>12</v>
       </c>
       <c r="F112" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="2:7">
       <c r="B113">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C113" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D113" t="s">
         <v>15</v>
@@ -2857,18 +2867,18 @@
         <v>12</v>
       </c>
       <c r="F113" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114" spans="2:7">
       <c r="B114">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C114" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D114" t="s">
         <v>15</v>
@@ -2877,7 +2887,7 @@
         <v>12</v>
       </c>
       <c r="F114" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>129</v>
@@ -2885,10 +2895,10 @@
     </row>
     <row r="115" spans="2:7">
       <c r="B115">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D115" t="s">
         <v>15</v>
@@ -2897,18 +2907,18 @@
         <v>12</v>
       </c>
       <c r="F115" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="116" spans="2:7">
       <c r="B116">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C116" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
@@ -2917,18 +2927,18 @@
         <v>12</v>
       </c>
       <c r="F116" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="2:7">
       <c r="B117">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D117" t="s">
         <v>15</v>
@@ -2937,59 +2947,79 @@
         <v>12</v>
       </c>
       <c r="F117" t="s">
-        <v>31</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="118" spans="2:7">
       <c r="B118">
+        <v>114</v>
+      </c>
+      <c r="C118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118" t="s">
+        <v>31</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119">
         <v>115</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>36</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D119" t="s">
         <v>11</v>
       </c>
-      <c r="E118" t="s">
-        <v>12</v>
-      </c>
-      <c r="F118" t="s">
+      <c r="E119" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="30">
-      <c r="B119">
+    <row r="120" spans="2:7" ht="45">
+      <c r="B120">
         <v>116</v>
       </c>
-      <c r="C119" t="s">
-        <v>134</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="C120" t="s">
+        <v>131</v>
+      </c>
+      <c r="D120" t="s">
         <v>51</v>
       </c>
-      <c r="E119" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" t="s">
+      <c r="E120" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" t="s">
         <v>49</v>
       </c>
-      <c r="G119" s="2" t="s">
-        <v>50</v>
+      <c r="G120" s="8" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G25" r:id="rId1"/>
-    <hyperlink ref="G43" r:id="rId2"/>
-    <hyperlink ref="G48" r:id="rId3"/>
-    <hyperlink ref="G66" r:id="rId4"/>
-    <hyperlink ref="G77" r:id="rId5"/>
-    <hyperlink ref="G95" r:id="rId6"/>
-    <hyperlink ref="G99" r:id="rId7"/>
-    <hyperlink ref="G117" r:id="rId8"/>
+    <hyperlink ref="G26" r:id="rId1"/>
+    <hyperlink ref="G44" r:id="rId2"/>
+    <hyperlink ref="G49" r:id="rId3"/>
+    <hyperlink ref="G67" r:id="rId4"/>
+    <hyperlink ref="G78" r:id="rId5"/>
+    <hyperlink ref="G96" r:id="rId6"/>
+    <hyperlink ref="G100" r:id="rId7"/>
+    <hyperlink ref="G118" r:id="rId8"/>
     <hyperlink ref="G3" r:id="rId9"/>
     <hyperlink ref="G21" r:id="rId10"/>
   </hyperlinks>
@@ -3043,12 +3073,12 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -3071,16 +3101,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3088,16 +3118,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3105,16 +3135,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
@@ -3122,16 +3152,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3139,16 +3169,16 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3156,16 +3186,16 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3223,12 +3253,12 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -3237,13 +3267,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3251,19 +3281,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
@@ -3273,13 +3303,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3287,18 +3317,18 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -3307,13 +3337,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3321,13 +3351,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3394,7 +3424,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3402,7 +3432,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -3416,7 +3446,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -3425,7 +3455,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3433,19 +3463,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3453,16 +3483,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3470,16 +3500,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3487,21 +3517,21 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3509,13 +3539,13 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3523,7 +3553,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -3532,7 +3562,7 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3540,19 +3570,19 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
         <v>86</v>
       </c>
-      <c r="D12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>87</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3560,16 +3590,16 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3577,16 +3607,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3594,21 +3624,21 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3616,13 +3646,13 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3630,7 +3660,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
         <v>51</v>
@@ -3639,10 +3669,10 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3650,7 +3680,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -3659,7 +3689,7 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3667,19 +3697,19 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3687,19 +3717,19 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3707,16 +3737,16 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3724,16 +3754,16 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3741,16 +3771,16 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3758,13 +3788,13 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1">
@@ -3772,7 +3802,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
@@ -3781,15 +3811,15 @@
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16" customHeight="1">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1">
@@ -3797,7 +3827,7 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -3806,7 +3836,7 @@
         <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16" customHeight="1">
@@ -3814,19 +3844,19 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
         <v>51</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3834,19 +3864,19 @@
         <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -3854,16 +3884,16 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3871,16 +3901,16 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3902,17 +3932,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="29.83203125" customWidth="1"/>
     <col min="7" max="7" width="36.6640625" customWidth="1"/>
   </cols>
@@ -3942,7 +3972,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -3951,7 +3981,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -3965,19 +3995,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>99</v>
       </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3985,91 +4015,97 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7">
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
         <v>99</v>
       </c>
-      <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7">
       <c r="B11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>9</v>
@@ -4077,54 +4113,46 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="G12" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="C14" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>57</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Not sure what I changed just want the latest up there
</commit_message>
<xml_diff>
--- a/testcases/KeywordDrivenFramework-2.xlsx
+++ b/testcases/KeywordDrivenFramework-2.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-31280" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="ContactUs" sheetId="1" r:id="rId1"/>
+    <sheet name="Contact_Us" sheetId="1" r:id="rId1"/>
     <sheet name="Mobile_Contact" sheetId="3" r:id="rId2"/>
     <sheet name="Verify_SSL" sheetId="5" r:id="rId3"/>
-    <sheet name="Location Finder" sheetId="8" r:id="rId4"/>
+    <sheet name="Location_Finder" sheetId="8" r:id="rId4"/>
     <sheet name="Search" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="152">
   <si>
     <t>TCName</t>
   </si>
@@ -331,12 +331,6 @@
     <t>CA Search</t>
   </si>
   <si>
-    <t>CA/FR Search</t>
-  </si>
-  <si>
-    <t>Uniformes</t>
-  </si>
-  <si>
     <t>sfsearchResultStatistics</t>
   </si>
   <si>
@@ -448,7 +442,43 @@
     <t>Verify Search Results Available CA</t>
   </si>
   <si>
-    <t>Verify Search Results Available CA/FR</t>
+    <t>Navigate to Cintas Staging CA Environment</t>
+  </si>
+  <si>
+    <t>takescreenshot</t>
+  </si>
+  <si>
+    <t>casearchresults</t>
+  </si>
+  <si>
+    <t>ussearchresults</t>
+  </si>
+  <si>
+    <t>ScreenShot CA Search</t>
+  </si>
+  <si>
+    <t>ScreenShot US Search</t>
+  </si>
+  <si>
+    <t>contactus_ca_fr</t>
+  </si>
+  <si>
+    <t>contactus_us</t>
+  </si>
+  <si>
+    <t>mobile_view</t>
+  </si>
+  <si>
+    <t>french_invalidlocation</t>
+  </si>
+  <si>
+    <t>french_validlocation</t>
+  </si>
+  <si>
+    <t>ca_validlocation</t>
+  </si>
+  <si>
+    <t>us_validlocation</t>
   </si>
 </sst>
 </file>
@@ -878,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G24" sqref="C24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -915,12 +945,12 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -934,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1185,7 +1215,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1205,7 +1235,7 @@
         <v>25</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1225,7 +1255,7 @@
         <v>26</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1290,7 +1320,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
@@ -1302,7 +1332,7 @@
         <v>49</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1310,10 +1340,13 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1437,7 +1470,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="2:10">
       <c r="B33">
         <v>29</v>
       </c>
@@ -1454,7 +1487,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="2:10">
       <c r="B34">
         <v>30</v>
       </c>
@@ -1472,7 +1505,7 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="2:10">
       <c r="B35">
         <v>31</v>
       </c>
@@ -1490,7 +1523,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="2:10">
       <c r="B36">
         <v>32</v>
       </c>
@@ -1507,7 +1540,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="2:10">
       <c r="B37">
         <v>33</v>
       </c>
@@ -1527,7 +1560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="2:10">
       <c r="B38">
         <v>34</v>
       </c>
@@ -1547,7 +1580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="2:10">
       <c r="B39">
         <v>35</v>
       </c>
@@ -1567,7 +1600,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="2:10">
       <c r="B40">
         <v>36</v>
       </c>
@@ -1584,10 +1617,10 @@
         <v>18</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
       <c r="B41">
         <v>37</v>
       </c>
@@ -1607,7 +1640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="2:10">
       <c r="B42">
         <v>38</v>
       </c>
@@ -1627,7 +1660,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="2:10">
       <c r="B43">
         <v>39</v>
       </c>
@@ -1647,7 +1680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="2:10">
       <c r="B44">
         <v>40</v>
       </c>
@@ -1667,7 +1700,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="2:10">
       <c r="B45">
         <v>41</v>
       </c>
@@ -1684,7 +1717,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="2:10">
       <c r="B46">
         <v>42</v>
       </c>
@@ -1701,12 +1734,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="30">
+    <row r="47" spans="2:10" ht="30">
       <c r="B47">
         <v>43</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
         <v>51</v>
@@ -1721,68 +1754,62 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" t="s">
+    <row r="48" spans="2:10">
+      <c r="C48" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
         <v>52</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
-      <c r="B49">
+    <row r="50" spans="1:7">
+      <c r="B50">
         <v>45</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>8</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
-      <c r="B50">
+    <row r="51" spans="1:7">
+      <c r="B51">
         <v>46</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>10</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>11</v>
       </c>
-      <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
-      <c r="B51">
+    <row r="52" spans="1:7">
+      <c r="B52">
         <v>47</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>39</v>
-      </c>
-      <c r="D51" t="s">
-        <v>38</v>
-      </c>
-      <c r="E51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7">
-      <c r="B52">
-        <v>48</v>
-      </c>
-      <c r="C52" t="s">
-        <v>40</v>
       </c>
       <c r="D52" t="s">
         <v>38</v>
@@ -1791,15 +1818,15 @@
         <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="B53">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
         <v>38</v>
@@ -1808,15 +1835,15 @@
         <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="B54">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D54" t="s">
         <v>38</v>
@@ -1825,15 +1852,15 @@
         <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="B55">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
         <v>38</v>
@@ -1842,15 +1869,15 @@
         <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="B56">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D56" t="s">
         <v>38</v>
@@ -1859,15 +1886,15 @@
         <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="B57">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D57" t="s">
         <v>38</v>
@@ -1876,15 +1903,15 @@
         <v>12</v>
       </c>
       <c r="F57" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="B58">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D58" t="s">
         <v>38</v>
@@ -1893,133 +1920,130 @@
         <v>12</v>
       </c>
       <c r="F58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="B59">
+        <v>54</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
         <v>31</v>
       </c>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="2:7">
-      <c r="B59">
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="B60">
         <v>55</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>35</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>11</v>
       </c>
-      <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="2:7">
-      <c r="B60">
+    <row r="61" spans="1:7">
+      <c r="B61">
         <v>56</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>14</v>
       </c>
-      <c r="D60" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
         <v>16</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="2:7">
-      <c r="B61">
+    <row r="62" spans="1:7">
+      <c r="B62">
         <v>57</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>19</v>
       </c>
-      <c r="D61" t="s">
-        <v>15</v>
-      </c>
-      <c r="E61" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" t="s">
         <v>20</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="2:7">
-      <c r="B62">
+    <row r="63" spans="1:7">
+      <c r="B63">
         <v>58</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>43</v>
       </c>
-      <c r="D62" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
         <v>42</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="2:7">
-      <c r="B63">
+    <row r="64" spans="1:7">
+      <c r="B64">
         <v>59</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>17</v>
       </c>
-      <c r="D63" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
         <v>18</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7">
-      <c r="B64">
-        <v>60</v>
-      </c>
-      <c r="C64" t="s">
-        <v>24</v>
-      </c>
-      <c r="D64" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" t="s">
-        <v>25</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="B65">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s">
         <v>15</v>
@@ -2028,18 +2052,18 @@
         <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>26</v>
-      </c>
-      <c r="G65" s="2">
-        <v>45324</v>
+        <v>25</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="B66">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -2048,18 +2072,18 @@
         <v>12</v>
       </c>
       <c r="F66" t="s">
-        <v>29</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
+      </c>
+      <c r="G66" s="2">
+        <v>45324</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="B67">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D67" t="s">
         <v>15</v>
@@ -2068,35 +2092,38 @@
         <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>31</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="B68">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
       </c>
       <c r="F68" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -2105,32 +2132,32 @@
         <v>12</v>
       </c>
       <c r="F69" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="B70">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D70" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E70" t="s">
         <v>12</v>
       </c>
       <c r="F70" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="B71">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D71" t="s">
         <v>38</v>
@@ -2139,35 +2166,32 @@
         <v>12</v>
       </c>
       <c r="F71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="B72">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E72" t="s">
         <v>12</v>
       </c>
       <c r="F72" t="s">
-        <v>25</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="B73">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D73" t="s">
         <v>15</v>
@@ -2176,122 +2200,125 @@
         <v>12</v>
       </c>
       <c r="F73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="B74">
+        <v>69</v>
+      </c>
+      <c r="C74" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="B75">
         <v>70</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>56</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>11</v>
       </c>
-      <c r="E74" t="s">
-        <v>12</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30">
-      <c r="B75">
+    <row r="76" spans="1:7" ht="30">
+      <c r="B76">
         <v>71</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" t="s">
+        <v>49</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77">
+        <v>72</v>
+      </c>
+      <c r="C77" t="s">
         <v>134</v>
       </c>
-      <c r="D75" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" t="s">
-        <v>12</v>
-      </c>
-      <c r="F75" t="s">
-        <v>49</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="B76">
-        <v>72</v>
-      </c>
-      <c r="C76" t="s">
-        <v>136</v>
-      </c>
-      <c r="D76" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>125</v>
-      </c>
-      <c r="B77">
+      <c r="D77" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78">
         <v>73</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="B78">
-        <v>74</v>
-      </c>
-      <c r="C78" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" t="s">
-        <v>9</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="B79">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="B80">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E80" t="s">
         <v>12</v>
       </c>
       <c r="F80" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="2:7">
       <c r="B81">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D81" t="s">
         <v>38</v>
@@ -2300,15 +2327,15 @@
         <v>12</v>
       </c>
       <c r="F81" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="2:7">
       <c r="B82">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D82" t="s">
         <v>38</v>
@@ -2317,15 +2344,15 @@
         <v>12</v>
       </c>
       <c r="F82" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="2:7">
       <c r="B83">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D83" t="s">
         <v>38</v>
@@ -2334,15 +2361,15 @@
         <v>12</v>
       </c>
       <c r="F83" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="2:7">
       <c r="B84">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D84" t="s">
         <v>38</v>
@@ -2351,15 +2378,15 @@
         <v>12</v>
       </c>
       <c r="F84" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="2:7">
       <c r="B85">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D85" t="s">
         <v>38</v>
@@ -2368,15 +2395,15 @@
         <v>12</v>
       </c>
       <c r="F85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="2:7">
       <c r="B86">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D86" t="s">
         <v>38</v>
@@ -2385,15 +2412,15 @@
         <v>12</v>
       </c>
       <c r="F86" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="2:7">
       <c r="B87">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D87" t="s">
         <v>38</v>
@@ -2402,53 +2429,50 @@
         <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>31</v>
-      </c>
-      <c r="G87" s="3"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="88" spans="2:7">
       <c r="B88">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D88" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E88" t="s">
         <v>12</v>
       </c>
       <c r="F88" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G88" s="3"/>
     </row>
     <row r="89" spans="2:7">
       <c r="B89">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D89" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E89" t="s">
         <v>12</v>
       </c>
       <c r="F89" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="90" spans="2:7">
       <c r="B90">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D90" t="s">
         <v>15</v>
@@ -2457,18 +2481,18 @@
         <v>12</v>
       </c>
       <c r="F90" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="2:7">
       <c r="B91">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C91" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D91" t="s">
         <v>15</v>
@@ -2477,18 +2501,18 @@
         <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="2:7">
       <c r="B92">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C92" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D92" t="s">
         <v>15</v>
@@ -2497,18 +2521,18 @@
         <v>12</v>
       </c>
       <c r="F92" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93" spans="2:7">
       <c r="B93">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C93" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D93" t="s">
         <v>15</v>
@@ -2517,18 +2541,18 @@
         <v>12</v>
       </c>
       <c r="F93" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="2:7">
       <c r="B94">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C94" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D94" t="s">
         <v>15</v>
@@ -2537,18 +2561,18 @@
         <v>12</v>
       </c>
       <c r="F94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="2:7">
       <c r="B95">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D95" t="s">
         <v>15</v>
@@ -2557,18 +2581,18 @@
         <v>12</v>
       </c>
       <c r="F95" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="2:7">
       <c r="B96">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D96" t="s">
         <v>15</v>
@@ -2577,111 +2601,114 @@
         <v>12</v>
       </c>
       <c r="F96" t="s">
-        <v>31</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="B97">
+        <v>92</v>
+      </c>
+      <c r="C97" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" t="s">
+        <v>31</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="B98">
         <v>93</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>36</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>11</v>
       </c>
-      <c r="E97" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="30">
-      <c r="B98">
+    <row r="99" spans="1:7" ht="30">
+      <c r="B99">
         <v>94</v>
       </c>
-      <c r="C98" t="s">
-        <v>132</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C99" t="s">
+        <v>130</v>
+      </c>
+      <c r="D99" t="s">
         <v>51</v>
       </c>
-      <c r="E98" t="s">
-        <v>12</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E99" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" t="s">
         <v>49</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>128</v>
-      </c>
-      <c r="B99">
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>126</v>
+      </c>
+      <c r="B100">
         <v>95</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="B100">
-        <v>96</v>
-      </c>
-      <c r="C100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100" t="s">
-        <v>9</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="B101">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>11</v>
-      </c>
-      <c r="E101" t="s">
-        <v>12</v>
-      </c>
-      <c r="F101" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="B102">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E102" t="s">
         <v>12</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="B103">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D103" t="s">
         <v>38</v>
@@ -2690,15 +2717,15 @@
         <v>12</v>
       </c>
       <c r="F103" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="B104">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C104" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D104" t="s">
         <v>38</v>
@@ -2707,15 +2734,15 @@
         <v>12</v>
       </c>
       <c r="F104" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="B105">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C105" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D105" t="s">
         <v>38</v>
@@ -2724,15 +2751,15 @@
         <v>12</v>
       </c>
       <c r="F105" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="B106">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D106" t="s">
         <v>38</v>
@@ -2741,15 +2768,15 @@
         <v>12</v>
       </c>
       <c r="F106" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="B107">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C107" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D107" t="s">
         <v>38</v>
@@ -2758,15 +2785,15 @@
         <v>12</v>
       </c>
       <c r="F107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="B108">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D108" t="s">
         <v>38</v>
@@ -2775,15 +2802,15 @@
         <v>12</v>
       </c>
       <c r="F108" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="B109">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C109" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D109" t="s">
         <v>38</v>
@@ -2792,53 +2819,50 @@
         <v>12</v>
       </c>
       <c r="F109" t="s">
-        <v>31</v>
-      </c>
-      <c r="G109" s="3"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="110" spans="1:7">
       <c r="B110">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C110" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D110" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E110" t="s">
         <v>12</v>
       </c>
       <c r="F110" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G110" s="3"/>
     </row>
     <row r="111" spans="1:7">
       <c r="B111">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C111" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D111" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E111" t="s">
         <v>12</v>
       </c>
       <c r="F111" t="s">
-        <v>16</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="B112">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C112" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D112" t="s">
         <v>15</v>
@@ -2847,18 +2871,18 @@
         <v>12</v>
       </c>
       <c r="F112" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="2:7">
       <c r="B113">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C113" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D113" t="s">
         <v>15</v>
@@ -2867,18 +2891,18 @@
         <v>12</v>
       </c>
       <c r="F113" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="2:7">
       <c r="B114">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C114" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D114" t="s">
         <v>15</v>
@@ -2887,18 +2911,18 @@
         <v>12</v>
       </c>
       <c r="F114" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
     </row>
     <row r="115" spans="2:7">
       <c r="B115">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C115" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D115" t="s">
         <v>15</v>
@@ -2907,18 +2931,18 @@
         <v>12</v>
       </c>
       <c r="F115" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" spans="2:7">
       <c r="B116">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C116" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
@@ -2927,18 +2951,18 @@
         <v>12</v>
       </c>
       <c r="F116" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="117" spans="2:7">
       <c r="B117">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C117" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D117" t="s">
         <v>15</v>
@@ -2947,18 +2971,18 @@
         <v>12</v>
       </c>
       <c r="F117" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
     </row>
     <row r="118" spans="2:7">
       <c r="B118">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C118" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D118" t="s">
         <v>15</v>
@@ -2967,59 +2991,79 @@
         <v>12</v>
       </c>
       <c r="F118" t="s">
-        <v>31</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="119" spans="2:7">
       <c r="B119">
+        <v>114</v>
+      </c>
+      <c r="C119" t="s">
+        <v>30</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" t="s">
+        <v>31</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120">
         <v>115</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>36</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D120" t="s">
         <v>11</v>
       </c>
-      <c r="E119" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" t="s">
+      <c r="E120" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="45">
-      <c r="B120">
+    <row r="121" spans="2:7" ht="45">
+      <c r="B121">
         <v>116</v>
       </c>
-      <c r="C120" t="s">
-        <v>131</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="C121" t="s">
+        <v>129</v>
+      </c>
+      <c r="D121" t="s">
         <v>51</v>
       </c>
-      <c r="E120" t="s">
-        <v>12</v>
-      </c>
-      <c r="F120" t="s">
+      <c r="E121" t="s">
+        <v>12</v>
+      </c>
+      <c r="F121" t="s">
         <v>49</v>
       </c>
-      <c r="G120" s="8" t="s">
-        <v>137</v>
+      <c r="G121" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G26" r:id="rId1"/>
     <hyperlink ref="G44" r:id="rId2"/>
-    <hyperlink ref="G49" r:id="rId3"/>
-    <hyperlink ref="G67" r:id="rId4"/>
-    <hyperlink ref="G78" r:id="rId5"/>
-    <hyperlink ref="G96" r:id="rId6"/>
-    <hyperlink ref="G100" r:id="rId7"/>
-    <hyperlink ref="G118" r:id="rId8"/>
+    <hyperlink ref="G50" r:id="rId3"/>
+    <hyperlink ref="G68" r:id="rId4"/>
+    <hyperlink ref="G79" r:id="rId5"/>
+    <hyperlink ref="G97" r:id="rId6"/>
+    <hyperlink ref="G101" r:id="rId7"/>
+    <hyperlink ref="G119" r:id="rId8"/>
     <hyperlink ref="G3" r:id="rId9"/>
     <hyperlink ref="G21" r:id="rId10"/>
   </hyperlinks>
@@ -3035,10 +3079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3078,7 +3122,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -3196,6 +3240,22 @@
       </c>
       <c r="F9" s="6" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3258,7 +3318,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -3281,7 +3341,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
         <v>74</v>
@@ -3293,7 +3353,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
@@ -3317,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
         <v>74</v>
@@ -3328,7 +3388,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -3351,7 +3411,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
@@ -3384,10 +3444,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3424,7 +3484,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3530,248 +3590,240 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>117</v>
+      <c r="C9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>96</v>
+      <c r="A10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>84</v>
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>86</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
         <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
         <v>67</v>
       </c>
       <c r="F15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>118</v>
-      </c>
-    </row>
     <row r="17" spans="1:7">
-      <c r="B17">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>105</v>
+      <c r="C17" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>108</v>
+      <c r="A18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>84</v>
+        <v>9</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
         <v>67</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>107</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="B23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="B24">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
         <v>62</v>
@@ -3780,57 +3832,66 @@
         <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="B25">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>82</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="16" customHeight="1">
-      <c r="B26">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="16" customHeight="1">
-      <c r="A27" t="s">
-        <v>119</v>
+      <c r="G27" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1">
       <c r="B28">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -3838,87 +3899,138 @@
       <c r="F28" t="s">
         <v>84</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="16" customHeight="1">
-      <c r="B29">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="C29" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16" customHeight="1">
+      <c r="A30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16" customHeight="1">
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
         <v>111</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="B30">
-        <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="B31">
-        <v>27</v>
-      </c>
-      <c r="C31" t="s">
-        <v>89</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16" customHeight="1">
       <c r="B32">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
         <v>67</v>
       </c>
       <c r="F32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="C36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G10" r:id="rId2"/>
-    <hyperlink ref="G17" r:id="rId3" display="https://cintas-stage-ca.willin.gs"/>
-    <hyperlink ref="G25" r:id="rId4" display="https://cintas-stage-ca.willin.gs"/>
+    <hyperlink ref="G11" r:id="rId2"/>
+    <hyperlink ref="G19" r:id="rId3" display="https://cintas-stage-ca.willin.gs"/>
+    <hyperlink ref="G27" r:id="rId4" display="https://cintas-stage-ca.willin.gs"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3932,10 +4044,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4015,7 +4127,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
@@ -4024,52 +4136,47 @@
         <v>12</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
       <c r="B6">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
       <c r="F6" s="7"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4077,88 +4184,57 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="2"/>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>102</v>
-      </c>
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7">
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="C11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" t="s">
         <v>141</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G7" r:id="rId2"/>
-    <hyperlink ref="G11" r:id="rId3"/>
+    <hyperlink ref="G8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>